<commit_message>
adding more products exp
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -314,6 +314,111 @@
   </si>
   <si>
     <t xml:space="preserve">https://imgmarketplace.lojasrenner.com.br/20000/3651/7010701763611/7510703532927/0.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camicado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colocação de papel de parede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580002/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colocação de piso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580003/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material para reforma de ambiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580004/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalação de portas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580012/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conjunto malas para viagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580016/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestador de serviços residenciais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580018/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pintura ambiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580019/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula de Valsa para os Noivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580029/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia da noiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580041/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massagem com pedras quentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580050/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massagem relaxante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580052/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diária em Hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580059/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diária em pousada no campo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580062/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transporte para Mudança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580079/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula de Culinária</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580092/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enxoval de lingerie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580105/small/1.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almoço no centro da cidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://img.camicado.com.br/item/sku580138/small/1.jpg</t>
   </si>
 </sst>
 </file>
@@ -447,13 +552,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H53" activeCellId="0" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.63"/>
@@ -1410,6 +1515,397 @@
         <v>39</v>
       </c>
     </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>200.0012</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>300.0013</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>400.0014</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>300.0013</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>450.00145</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>200.0012</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>300.0013</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>180.00118</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>800.0018</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>120.00112</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>90.0019</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>180.00118</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>150.00115</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>300.0013</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>100.0011</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>400.0014</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>140.00114</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" display="https://3a36cfaa62ac8ba9.cdn.gocache.net/images/produtos/sidney_brike1_20180606__g.jpg"/>

</xml_diff>